<commit_message>
Updated internal codesets with macrons lost in transfer from Word to CSV
</commit_message>
<xml_diff>
--- a/xlsx/health-research-council-theme.xlsx
+++ b/xlsx/health-research-council-theme.xlsx
@@ -53,10 +53,10 @@
     <t xml:space="preserve">RHM</t>
   </si>
   <si>
-    <t xml:space="preserve">Rangahau Hauora Maori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supporting Maori health research that upholds rangatiratanga and uses and advances Maori knowledge, resources and people</t>
+    <t xml:space="preserve">Rangahau Hauora Māori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supporting Māori health research that upholds rangatiratanga and uses and advances Māori knowledge, resources and people</t>
   </si>
 </sst>
 </file>

</xml_diff>